<commit_message>
Added a new updated file.
</commit_message>
<xml_diff>
--- a/Process Map.xlsx
+++ b/Process Map.xlsx
@@ -1148,73 +1148,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>391886</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>108857</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>468085</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>174172</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Rectangle 49"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1001486" y="10678886"/>
-          <a:ext cx="3733799" cy="990600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>Predictive Analysis</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-IN" sz="1100"/>
-            <a:t> Brand maeketing experiments to check</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-IN" sz="1100" baseline="0"/>
-            <a:t> if it is finacially and emotionally suitable to market the brand</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-IN" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -3201,7 +3134,7 @@
   <dimension ref="B21:U111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE48" sqref="AE48"/>
+      <selection activeCell="AD69" sqref="AD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>